<commit_message>
only user data in xlsx
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>s_no</t>
   </si>
@@ -34,28 +34,16 @@
     <t>verify_otp</t>
   </si>
   <si>
-    <t>kenil</t>
-  </si>
-  <si>
-    <t>kenilmangroliya18@gmail.com</t>
-  </si>
-  <si>
-    <t>$2b$10$WeKNghEFVP0KC0wIstceAOgXbQ49RBunZGGPH3.miMpbaVahH1cXa</t>
-  </si>
-  <si>
-    <t>/public/images/2.jpg</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>admin@gmail.com</t>
-  </si>
-  <si>
-    <t>$2b$10$d1FY7Dtn1kf.ah2v58/PV.gVaqITpLhFGSU4KIkf0EekpoGIM2tSi</t>
-  </si>
-  <si>
-    <t>image/png</t>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>aa@gmail.com</t>
+  </si>
+  <si>
+    <t>$2b$10$aMWseoSQNXof5F78tCDz6uN.xy/U1H3cvPRaPbjGKw0/NsjlvE55O</t>
+  </si>
+  <si>
+    <t>/public/images/4.jpg</t>
   </si>
 </sst>
 </file>
@@ -436,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="10" customWidth="1"/>
@@ -482,29 +470,9 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1397</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>